<commit_message>
Added bash script to run site
</commit_message>
<xml_diff>
--- a/outline_testing/map_test_data.xlsx
+++ b/outline_testing/map_test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Ellison\Desktop\CodeForGood\outline_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9297D475-FE37-460D-922A-F5B2D4FD115D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9A0EF-4A0F-4132-BB6D-77666D3B63F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{D5CD3BF6-7BDC-4B99-BDC7-1E82915A4C9A}"/>
   </bookViews>
@@ -2963,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE39C63-2E3D-4C18-AAF5-D0A4B6862FF8}">
-  <dimension ref="A1:D352"/>
+  <dimension ref="A1:H352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2977,7 +2977,7 @@
     <col min="4" max="4" width="29.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2999,13 +2999,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1234</v>
+        <v>1923232839</v>
       </c>
       <c r="D2">
         <v>22498</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="H2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3019,7 +3022,7 @@
         <v>29649</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -3033,7 +3036,7 @@
         <v>21344</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>29035</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -3061,7 +3064,7 @@
         <v>25239</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -3075,7 +3078,7 @@
         <v>24364</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>29250</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -3103,7 +3106,7 @@
         <v>23439</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>25323</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>26610</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>24955</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -3159,7 +3162,7 @@
         <v>22488</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>26633</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>22455</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>

</xml_diff>